<commit_message>
some minor errors in numbering etc
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -20100,6 +20100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -20188,25 +20189,25 @@
   <dimension ref="A1:P1133"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="209.97"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="5" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="209.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="167.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="210.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changed the definition of SKIN to disambiguate between two Avar words (possibly in other languages too)
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -4471,10 +4471,10 @@
     <t xml:space="preserve">SKIN</t>
   </si>
   <si>
-    <t xml:space="preserve">Кожа человека. (GLD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human skin. (GLD)</t>
+    <t xml:space="preserve">Кожа человека. (GLD) Если в языке есть и общее слово для кожи, в том числе используемой как материал, и специальное слово для кожи на теле человека (ср. авар. &lt;i&gt;къехь&lt;/i&gt; vs. &lt;i&gt;тІом&lt;/i&gt;), сюда вводится второе.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human skin. (GLD) If the language has separate words for skin in general (including skin used as material) and human skin on the body (cf. Avar &lt;i&gt;qʼexː&lt;/i&gt; vs. &lt;i&gt;tʼom&lt;/i&gt;), the latter should be entered.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Я порезал свою кожу. (GLD) 2. Под кожей человека мышцы и кости. </t>
@@ -20100,7 +20100,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -20189,25 +20188,25 @@
   <dimension ref="A1:P1133"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:H"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.25"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="5" style="0" width="4.07"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="209.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="209.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="167.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="210.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated definitions for two types of HIDE
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -4489,7 +4489,7 @@
     <t xml:space="preserve">HIDE OF GOATS AND SHEEP</t>
   </si>
   <si>
-    <t xml:space="preserve">Шкура овец и коз.</t>
+    <t xml:space="preserve">Шкура овец и коз. В отличие от 250 КОЖА, здесь нужно выбирать слово, способное обозначать кожу как материал (см. контексты).</t>
   </si>
   <si>
     <t xml:space="preserve">The hide of goats and sheep.</t>
@@ -4507,7 +4507,7 @@
     <t xml:space="preserve">HIDE OF COWS</t>
   </si>
   <si>
-    <t xml:space="preserve">Шкура коров.</t>
+    <t xml:space="preserve">Шкура коров. Unlike 250 SKIN, the word chosen here should be able to denote skin as a material (see contexts).</t>
   </si>
   <si>
     <t xml:space="preserve">The hide of cows.</t>
@@ -20187,8 +20187,8 @@
   </sheetPr>
   <dimension ref="A1:P1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A236" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A252" activeCellId="0" sqref="A252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Specified that 151 RAM must be uncastrated
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Наиболее общее слово для материала, состоящего из мелких частиц минералов, ракушек, камней и т.д., различимых невооружённым глазом. Избегать терминов для специальных видов или цветов песка. Избегать слов для ‘пыли’, ‘грязи’ и относящиеся к типу почвы, а не к самому материалу. Не использовать слов для ‘пляжа’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for the loose material consisting of small particles of mineral, shell, rock etc., distinguishable by the naked eye. Avoid terms for specific types or colour of sand. Avoid terms referring to "dust" or "dirt", where different. Avoid terms referring to soil type, where different. Avoid terms referring specifically to "beach" or "strand". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for the loose material consisting of small particles of mineral, shell, rock etc., distinguishable by the naked eye. Avoid terms for specific types or colour of sand. Avoid terms referring to “dust” or “dirt”, where different. Avoid terms referring to soil type, where different. Avoid terms referring specifically to “beach” or “strand”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Она просыпала песок сквозь руки. (CoBL) 2. Он взял в горсть песка. (GLD) 3. Я не знаю, что на том участке: земля или песок. (GLD)</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">Наиболее общее существительное для существенного повышения ландшафта, как правило, с крутыми склонами. Избегать терминов для отдельных типов гор; меньших возвышений (‘холм’, ‘курган’); частей горы (‘вершина’). (CoBL)Если есть особое наречие ‘в горах’ или специальное выражение для гор «вообще», вводить их как неосновные синонимы.</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic substantive for a considerable rise in the surface of the Earth, typically with steep slopes. Avoid terms for specific types of mountain. Avoid terms for smaller rises, e.g. "mound, hill". Avoid terms for parts of a mountain, e.g. "peak". (CoBL)</t>
+    <t xml:space="preserve">Most generic substantive for a considerable rise in the surface of the Earth, typically with steep slopes. Avoid terms for specific types of mountain. Avoid terms for smaller rises, e.g. “mound, hill”. Avoid terms for parts of a mountain, e.g. “peak”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. В Дагестане есть равнина и много гор. 2. На эту гору подниматься целый день. (GLD)</t>
@@ -340,7 +340,7 @@
     <t xml:space="preserve">Самое общее слово для крупной массы солёной воды. Избегать слов для его частей, например, ‘бухта’, ‘залив’ и т.д. Не использовать скорее картографических терминов, как, например, ‘океан’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for a large body of salt water. Avoid terms for subsets thereof, e.g. "bay", "inlet" etc. Avoid more cartographical terminology, e.g. "ocean". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for a large body of salt water. Avoid terms for subsets thereof, e.g. “bay”, “inlet” etc. Avoid more cartographical terminology, e.g. “ocean”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Река спускается с гор и впадает в море. 2. Морская вода — солёная. </t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Нейтральное слово для потока свежей воды, текущего по углублению над землёй, обычно впадающего в озеро или море. Избегать терминов для маленьких или больших рек. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for a stream of fresh water flowing in a channel above the ground, often ending in a lake or in the sea. Avoid terms specifically for smaller, e.g. "stream", or larger, e.g. Fr. "fleuve", rivers. (CoBL)</t>
+    <t xml:space="preserve">Most generic term for a stream of fresh water flowing in a channel above the ground, often ending in a lake or in the sea. Avoid terms specifically for smaller, e.g. “stream”, or larger, e.g. Fr. “fleuve”, rivers. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Река течёт от гор к морю. 2. В нашей реке много рыбы.</t>
@@ -466,7 +466,7 @@
     <t xml:space="preserve">Самый общий термин для густого множества деревьев, покрывающего определённую местность. Отличать от специализированных терминов вроде «рощи». (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for a dense collection of trees and woody shrubs covering a certain area. Try to find the most generic term. English distinguishes between very small "copse", small to medium sized "woods" and large "forest". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for a dense collection of trees and woody shrubs covering a certain area. Try to find the most generic term. English distinguishes between very small ‘copse’, small to medium sized ‘woods’ and large ‘forest’. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. В лесу живут медведи. 2. В лесу много деревьев.</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">Самое общее слово для части земной атмосферы и пространства вне её, видимого с поверхности земли. В течение дня оно выглядит голубым, ночью — чёрным. Избегать религиозной терминологии (‘небеса’ и под.). (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic noun for the part of the earth's atmosphere and space outside it that is visible from earth's surface. During the day it is perceived as blue, and at night as black. Avoid religious terminology, e.g. "heaven(s)", where different. (CoBL)</t>
+    <t xml:space="preserve">Most generic noun for the part of the earth's atmosphere and space outside it that is visible from earth's surface. During the day it is perceived as blue, and at night as black. Avoid religious terminology, e.g. “heaven(s)”, where different. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">На голубом небе были белые облака. (CoBL)</t>
@@ -559,7 +559,7 @@
     <t xml:space="preserve">Самое общее слово для звезды в центре нашей солнечной системы, от которой Земля получает свет и тепло. Избегать терминов для ‘дневного времени’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for the particular star at the centre of our solar system, from which the Earth gets light and heat. Avoid terms specifically for "daytime", where different.  (CoBL)</t>
+    <t xml:space="preserve">Most generic term for the particular star at the centre of our solar system, from which the Earth gets light and heat. Avoid terms specifically for “daytime”, where different.  (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Ночью на небе видны звезды и луна, а днем солнце. (GLD) 2. Посмотри на солнце. (GLD)</t>
@@ -577,7 +577,7 @@
     <t xml:space="preserve">Самое общее слово для естественного спутника планеты Земля. Избегать слов для отдельных стадий луны, напр. ‘(полу)месяц’. Избегать слов, чьим основным значением является скорее единица времени ‘месяц’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for the satellite of the planet Earth. Avoid terms for specific stages of the moon, e.g. "crescent". Avoid words that refer primarily to the time-unit of a 'month'; the word entered should be the basic word for the celestial object. (CoBL)</t>
+    <t xml:space="preserve">Most generic term for the satellite of the planet Earth. Avoid terms for specific stages of the moon, e.g. “crescent”. Avoid words that refer primarily to the time-unit of a ‘month’; the word entered should be the basic word for the celestial object. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Днем светит солнце, а ночью — луна. 2. На небе круглая луна.</t>
@@ -775,7 +775,7 @@
     <t xml:space="preserve">Влажные осадки (общий термин). Избегать слов для отдельных видов дождя (‘ливень’, ‘грибной дождь’). (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for liquid precipitation. Avoid terms for different types of precipitation, e.g. "drizzle", or denoting duration, e.g. "shower". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for liquid precipitation. Avoid terms for different types of precipitation, e.g. “drizzle”, or denoting duration, e.g. “shower”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Дождь — это небесная вода. (GLD)  2. Посмотри на дождь, он пока еще не очень сильный. (GLD)</t>
@@ -1246,7 +1246,7 @@
     <t xml:space="preserve">Самое общее слово для взрослого человека женского пола. Избегать терминов родства и отношения там, где они отличаются. Избегать специальных слов для молодых или пожилых женщин. Избегать маркированных вежливых форм, таких, как ‘госпожа’ и т.д. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for an adult human female. Avoid relationship or kinship terms, where different. Avoid specific terms for younger or older women. Avoid honorific terms, e.g. "lady", etc. (CoBL)</t>
+    <t xml:space="preserve">Most generic term for an adult human female. Avoid relationship or kinship terms, where different. Avoid specific terms for younger or older women. Avoid honorific terms, e.g. “lady”, etc. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Мужчины делают [X], а женщины делают [Y]. (GLD) 2. Женщины рожают детей, а мужчины — нет. (GLD)</t>
@@ -2761,10 +2761,10 @@
     <t xml:space="preserve">RAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Взрослая особь овцы мужского пола.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adult male sheep.</t>
+    <t xml:space="preserve">Взрослая некастрированная особь овцы мужского пола.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult uncastrated male sheep.</t>
   </si>
   <si>
     <t xml:space="preserve">Баран не даёт молока, а овцематка — даёт.</t>
@@ -3178,7 +3178,7 @@
     <t xml:space="preserve">Самое общее слово для представителя класса птиц (&lt;i&gt;Aves&lt;/i&gt;). Когда это возможно, избегать специальных слов для больших, маленьких или хищных птиц. Избегать специальных слов для домашних птиц (ср. англ. &lt;i&gt;fowl&lt;/i&gt;).</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for a member of the class Aves. Avoid specific terms for a small, large or predatory bird where possible. Avoid terms for domesticated birds, i.e. "fowl".</t>
+    <t xml:space="preserve">Most generic term for a member of the class Aves. Avoid specific terms for a small, large or predatory bird where possible. Avoid terms for domesticated birds, i.e. “fowl”.</t>
   </si>
   <si>
     <t xml:space="preserve">1. В лесу поют птицы. 2. Птицы откладывают яйца. </t>
@@ -3472,7 +3472,7 @@
     <t xml:space="preserve">Самое общее слово для представителя вида &lt;i&gt;canis familiaris&lt;/i&gt;. Домашняя собака. Отличать от названий конкретных пород и специальных слов для собак определённого возраста или пола (‘щенок’, ‘сука’ и т.д.). (Kassian et al. 2010). Избегать названий охотничьих собак, напр. англ. &lt;i&gt;hound&lt;/i&gt;. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for animal of species canis familiaris. Domesticated dog. Not to be confused with various breeds or specific words for dogs of different ages or sexes (‘puppy’, ‘bitch’ etc.). (Kassian et al. 2010). Also, avoid terms for hunting dog, e.g. Eng. "hound". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for animal of species canis familiaris. Domesticated dog. Not to be confused with various breeds or specific words for dogs of different ages or sexes (‘puppy’, ‘bitch’ etc.). (Kassian et al. 2010). Also, avoid terms for hunting dog, e.g. Eng. “hound”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Собака охраняет овец. 2. Собака живёт с человеком, а дикие звери — нет.</t>
@@ -5200,7 +5200,7 @@
     <t xml:space="preserve">Базовое слово для человеческого глаза (орган зрения), но не специализированный медицинский или технический термин. Избегать слов для ‘зрения’ и под. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Basic term for human eye, but not specialised medical or technical terms if different. Avoid specific terms for "vision, sight" etc. (CoBL)</t>
+    <t xml:space="preserve">Basic term for human eye, but not specialised medical or technical terms if different. Avoid specific terms for ‘vision, sight’ etc. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. У человека бывает два глаза. 2. У него только один глаз. 3. Люди видят глазами.</t>
@@ -5419,7 +5419,7 @@
     <t xml:space="preserve">Базовое слово для языка человека (как органа); избегать специализированной терминологии. Не использовать специализированные слова для понятий ‘чувство вкуса’ или ‘язык’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Basic term for the human tongue, avoiding more technical anatomical terminology, if different. Avoid terms specific to "sense of taste" or "language" where possible. (CoBL)</t>
+    <t xml:space="preserve">Basic term for the human tongue, avoiding more technical anatomical terminology, if different. Avoid terms specific to ‘sense of taste’ or ‘language’ where possible. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он показал ему язык. (CoBL) 2. Когда он упал, он прикусил язык. Ему больно. (CoBL)</t>
@@ -6226,7 +6226,7 @@
     <t xml:space="preserve">BELLY</t>
   </si>
   <si>
-    <t xml:space="preserve">Часть туловища между грудью и пахом. Отличать от многочисленных внутренних органов (желудок, кишки и т. п.) и семантически/стилистически маркированных слов (пузо и т. п.)  (GLD)\</t>
+    <t xml:space="preserve">Часть туловища между грудью и пахом. Отличать от многочисленных внутренних органов (желудок, кишки и т. п.) и семантически/стилистически маркированных слов (пузо и т. п.)  (GLD)</t>
   </si>
   <si>
     <t xml:space="preserve">Part of the human body located directly above the pelvis. Not to be confused with various terms that denote internal organs (stomach, intestines) or semantically/stylistically marked words (paunch). (GLD)</t>
@@ -6589,7 +6589,7 @@
     <t xml:space="preserve">Самое общее слово для выпускания изо рта содержимого желудка. Во многих языках у этого слова проблема с нейтральным регистром. В таких слуаях выбирается самый общий термин, который может быть разговорным, но не является грубым. Если нет подходящего кандидата, используете более формальный термин. Для английского языка Сводешево слово для этого понятия не vomit, а throw up. В русском — «вырывать». (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for regurgitating the contents of the stomach. In many languages there is likely to be a problem in register with this word. In such cases, pick the most common term, which may be colloquial, but is not vulgar. If no suitable candidate exists, use the more formal term. The English Swadesh term for this meaning is probably not "vomit", but rather "throw up" in most varieties. (CoBL)</t>
+    <t xml:space="preserve">Most generic term for regurgitating the contents of the stomach. In many languages there is likely to be a problem in register with this word. In such cases, pick the most common term, which may be colloquial, but is not vulgar. If no suitable candidate exists, use the more formal term. The English Swadesh term for this meaning is probably not ‘vomit’, but rather ‘throw up’ in most varieties. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он съел что-то плохое, и его вырвало. (CoBL) 2. Если выпить слишком много водки, тебя вырвет.</t>
@@ -6673,7 +6673,7 @@
     <t xml:space="preserve">Самый общий глагол для отдыха в состоянии пониженного сознания и замедленного обмена веществ. По возможности стативное, а не динамическое или инхоативное значение (‘засыпать’), (CoBL) В дагестанских языках здесь часто возможен только инхоативный глагол — в таком случае надо вводить его формы СВ и НСВ в соответствующих полях, в столбце notes поставить «Inchoative verb».</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for resting in a state of decreased consciousness and reduced metabolism. Stative not dynamic or inchoative meaning, e.g. "fall asleep". (CoBL) In Daghestanian languages, often only an inchoative verb is available. In this case enter its pfv. and ipfv. forms in the corresponding fields, regardless of semantics, and put «Inchoative verb» in the notes column.</t>
+    <t xml:space="preserve">Most generic verb for resting in a state of decreased consciousness and reduced metabolism. Stative not dynamic or inchoative meaning, e.g. “fall asleep”. (CoBL) In Daghestanian languages, often only an inchoative verb is available. In this case enter its pfv. and ipfv. forms in the corresponding fields, regardless of semantics, and put “Inchoative verb” in the notes column.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Обычно ночью люди спят, а днем бодрствуют. (GLD) 2. Не буди его, он спит. (GLD)</t>
@@ -7645,7 +7645,7 @@
     <t xml:space="preserve">Самый общий глагол, обозначающий поглощение пищи человеком.Избегать маркированных глаголов («поедать», «поглощать»).Нейтральный регистр: избегать «детской» лексики, вежливых слов («кушать» и т.д.).Если в языке используются разные слова для разных видов еды (например, для мяса, круп, фруктов/орехов, твёрдой, мягкой, жидкой еды и т.д.), вводить самое нейтральное слово. Если такого слова нет, вводить глагол, используемый для самой базовой, традиционной пищи для носителей этого языка, например, рис, хлеб, кукуруза и т.д. (этот глагол также скорее всего окажется самым частотным) (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">The most generic verb for humans consuming food.Avoid marked verbs, e.g. "eat up, devour".Default register: avoid nursery words, polite words, etc.If your language uses different default words for different types of food (e.g. meat, cereals, fruits/nuts, hard food, soft food, liquid food, etc.), then enter the most generic word. If there is no such generic term, enter the verb used for eating the most basic, traditional foodstuff for most speakers of that language: e.g. rice, bread, maize, etc. (which will probably also be the most statistically frequent).  (CoBL)</t>
+    <t xml:space="preserve">The most generic verb for humans consuming food.Avoid marked verbs, e.g. “eat up, devour”.Default register: avoid nursery words, polite words, etc.If your language uses different default words for different types of food (e.g. meat, cereals, fruits/nuts, hard food, soft food, liquid food, etc.), then enter the most generic word. If there is no such generic term, enter the verb used for eating the most basic, traditional foodstuff for most speakers of that language: e.g. rice, bread, maize, etc. (which will probably also be the most statistically frequent).  (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Все люди едят хлеб. 2. Коровы едят траву. 3. Он съел обед.</t>
@@ -7753,7 +7753,7 @@
     <t xml:space="preserve">Самое общее прилагательное для разлагающейся или разложившейся твёрдой еды, как правило, фруктов. Постарайтесь избегать слов со значением ‘плесневелый’. Избегать специальных слов для мяса или разлагающейся плоти. Избегать специальных слов для дерева. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic adjective for decomposing or decomposed solid food, typically fruit. Try to avoid terms for "mouldy". Try to avoid terms specifically for meat or decomposing flesh. Try to avoid terms specifically for wood. (CoBL)</t>
+    <t xml:space="preserve">Most generic adjective for decomposing or decomposed solid food, typically fruit. Try to avoid terms for “mouldy”. Try to avoid terms specifically for meat or decomposing flesh. Try to avoid terms specifically for wood. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Это яблоко гнилое. (CoBL) 2. Не ешь гнилые фрукты.</t>
@@ -11761,7 +11761,7 @@
     <t xml:space="preserve">Самое общее слово для длинного, тонкого куска дерева, как правило, оставленного в той форме, в которой он рос, который не гнётся. (Concepticon) Избегать специальных слов для деревяшек, которыми разжигают огонь. Избегать слов для маленьких палок. (CoBL) Также не вводить слова для отдельных функциональных типов палок («посох»  и т.д.).</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for a long, thin piece of wood, mainly left in the shape in which it grew, that does not bend. (Concepticon) Avoid terms specifically used for starting a fire. Avoid terms for smaller sticks, e.g. "twigs". (CoBL) Also avoid terms for specific functional types of sticks, such as ‘staff’, etc.</t>
+    <t xml:space="preserve">Most generic term for a long, thin piece of wood, mainly left in the shape in which it grew, that does not bend. (Concepticon) Avoid terms specifically used for starting a fire. Avoid terms for smaller sticks, e.g. “twigs”. (CoBL) Also avoid terms for specific functional types of sticks, such as ‘staff’, etc.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он ударил собаку палкой. 2. Он подобрал с земли палку.</t>
@@ -12407,7 +12407,7 @@
     <t xml:space="preserve">Самый общий переходный глагол, относящийся к надрезыванию, а не отделению или разделению на части. Избегать слов со значением ‘отрезать’, ‘прорезать насквозь’, ‘разрезать пополам’, ‘разрезать на части’ и т.д. Избегать слов, относящихся специально к дереву. (CoBL) Включено для совместимости со списком Jena-200.</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic transitive verb referring to incision rather than separation or segmentation. Avoid terms for "cutting off", "cutting through", "cutting in half", "cut into pieces" etc. Avoid terms specific to cutting wood. (CoBL) Included for compatibility with the Jena 200 list.</t>
+    <t xml:space="preserve">Most generic transitive verb referring to incision rather than separation or segmentation. Avoid terms for “cutting off”, “cutting through”, “cutting in half”, “cut into pieces” etc. Avoid terms specific to cutting wood. (CoBL) Included for compatibility with the Jena 200 list.</t>
   </si>
   <si>
     <t xml:space="preserve">Я порезал палец: смотри, течёт кровь. (CoBL)</t>
@@ -12680,7 +12680,7 @@
     <t xml:space="preserve">Самый общий глагол для перемещения объекта с помощью рук в направлении к себе — базовый антоним глагола ‘толкать’. Избегать слов, обозначающих именно притягивание чего-то ближе к себе; выбранный глагол должен быть достаточно общим, чтобы включать в свой круг значений контекст, в которых человек, тянущий предмет, также двигается сам (т.е. тянет его вместе с собой). Избегать слов для волочения объекта в контакте с землёй; обозначающих резкое движение; эмфатических глаголов; глаголов, обозначающих вращение (например, ‘катить’), предполагающие, что объект уронили (англ. pull over) и прочие слишком частные значения. При этом следует также избегать более общего значения ‘двигать, нести’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for moving an object with the hands in a direction towards oneself -- basic opposite of 'push'.  Avoid terms specifically for bringing something closer to oneself; the verb selected should be generic enough also to apply to cases where the person pulling the object is himself moving, i.e. pulling it along. Avoid terms specifically for dragging an object in constant contact with the ground, e.g. 'drag', 'haul'. Avoid intensifying terms emphasising sudden pulling, e.g. 'yank'. Avoid intensifying terms emphasising strenuous force and/or particularly heavy objects, e.g. 'tug', "drag". Avoid terms specifically involving rotation (e.g. 'roll'), causing to fall (e.g. 'pull over') or other overly specific senses. Avoid terms for more general change of position, e.g. 'move, carry'. (CoBL)</t>
+    <t xml:space="preserve">Most generic verb for moving an object with the hands in a direction towards oneself -- basic opposite of ‘push’.  Avoid terms specifically for bringing something closer to oneself; the verb selected should be generic enough also to apply to cases where the person pulling the object is himself moving, i.e. pulling it along. Avoid terms specifically for dragging an object in constant contact with the ground, e.g. ‘drag’, ‘haul’. Avoid intensifying terms emphasising sudden pulling, e.g. ‘yank’. Avoid intensifying terms emphasising strenuous force and/or particularly heavy objects, e.g. ‘tug’, “drag”. Avoid terms specifically involving rotation (e.g. ‘roll’), causing to fall (e.g. ‘pull over’) or other overly specific senses. Avoid terms for more general change of position, e.g. ‘move, carry’. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он шёл и тянул за собой телегу. 2. Он потянул стол поближе к себе.</t>
@@ -12824,7 +12824,7 @@
     <t xml:space="preserve">Самый общий глагол для удаления грязи с тела человека. Избегать специальных слов для мытья одежды, посуды и т.д. Избегать слов для мытья с полным погружением, например ‘купать’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for removing dirt from the human body. Avoid specific terms for washing clothes, dishes etc. Avoid terms for total immersion, e.g. "bathe". (CoBL)</t>
+    <t xml:space="preserve">Most generic verb for removing dirt from the human body. Avoid specific terms for washing clothes, dishes etc. Avoid terms for total immersion, e.g. “bathe”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Она помыла руки. 2. Она моет посуду.</t>
@@ -13544,7 +13544,7 @@
     <t xml:space="preserve">Самый общий переходный глагол, обозначающий такой тип воздействия на объект, в результате которого меняется его ориентация относительно некоторой точки-ориентира. Использовать самое общее слово: избегать альтернативных выражений или дериватов (как английские фразовые глаголы или различные приставочные варианты) с более конкретными значениями, такими, как ‘перевернуть’, ‘повернуть’ и т.д., хотя они часто могут быть образованы от той же основы — по возможности использовать только самое простое, базовое слово. Требуется переходный глагол, поэтому следует избегать непереходных, рефлексивных глаголов, глаголов среднего залога и т.д. (опять же, многие из них будут образованы от того же корня, что и переходный глагол). Если язык использует разные слова для поворота в горизонтальной и вертикальной плоскости, использовать то, которое указывает на вращение в горизонтальной плоскости. Избегать слов только для частичных, только для полных или для многократных вращений. Если общего или полисемичного слова в языке нет, выбирайте то, которое обозначает вращение на 90 или 180 градусов — в зависимости от того, какой глагол является более простым в данном языке. Избегать технических терминов и слов со значением ‘скручивать’, ‘сплетать’ (ср. англ. twist). (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic transitive verb used for moving an object with the result that its orientation changes (relative to some reference point).  Select the most general term: avoid alternatives or derivatives (e.g. English phrasal verbs) with more specific meanings such as 'turn over', 'turn around', 'turn towards', 'orient', although these may often have similar stems - select only the default, most general term.  The transitive verb is needed, so avoid intransitives, reflexives, middles, etc. (many may of course share the same root as the transitive that is the target here, which is fine).  If your language uses different terms for turning in horizontal and vertical planes, then use the one prototypically for turning in the horizontal plane.  Avoid terms specifically for only partial, only complete, or multiple rotations. If there is no general cover or ambiguous term, select the one for 90 or 180 degree rotation, whichever is most basic in your language.  Avoid more technical terms, such as 'rotate', 'reorient', 'gyrate', etc..  Avoid specifically torsional movement, e.g. "twist". (CoBL)</t>
+    <t xml:space="preserve">Most generic transitive verb used for moving an object with the result that its orientation changes (relative to some reference point).  Select the most general term: avoid alternatives or derivatives (e.g. English phrasal verbs) with more specific meanings such as ‘turn over’, ‘turn around’, ‘turn towards’, ‘orient’, although these may often have similar stems - select only the default, most general term.  The transitive verb is needed, so avoid intransitives, reflexives, middles, etc. (many may of course share the same root as the transitive that is the target here, which is fine).  If your language uses different terms for turning in horizontal and vertical planes, then use the one prototypically for turning in the horizontal plane.  Avoid terms specifically for only partial, only complete, or multiple rotations. If there is no general cover or ambiguous term, select the one for 90 or 180 degree rotation, whichever is most basic in your language.  Avoid more technical terms, such as ‘rotate’, ‘reorient’, ‘gyrate’, etc..  Avoid specifically torsional movement, e.g. “twist”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Женщины крутят веретено. 2. Эта телега такая тяжёлая, что её трудно повернуть. (CoBL)</t>
@@ -13706,7 +13706,7 @@
     <t xml:space="preserve">Самый общий глагол, обозначающий движение людей ногами при ходьбе. Избегать глаголов, обозначающих скорость передвижения, например, ‘бежать’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for motion of human beings with the feet. Try to avoid specific terms denoting speed of movement, e.g. "run", etc. (CoBL)</t>
+    <t xml:space="preserve">Most generic verb for motion of human beings with the feet. Try to avoid specific terms denoting speed of movement, e.g. “run”, etc. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">Люди ходят, змеи ползают, птицы летают.</t>
@@ -13760,7 +13760,7 @@
     <t xml:space="preserve">Самый общий глагол для извергания воздуха с силой изо рта. Избегать форм, относящихся к дуновению ветра. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most basic verb for action of expelling air with force from the mouth. Avoid intransitive forms, such as the wind blowing. Avoid also blow in the sense of "hit". (CoBL)</t>
+    <t xml:space="preserve">Most basic verb for action of expelling air with force from the mouth. Avoid intransitive forms, such as the wind blowing. Avoid also blow in the sense of “hit”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он подул на палки, чтобы разжечь огонь. (CoBL) 2. Он подул на чай, чтобы тот остыл.</t>
@@ -13904,7 +13904,7 @@
     <t xml:space="preserve">Самый общий непереходный глагол для быстрого движения людей ногами. Избегать слов для движения жидкостей, там, где это отдельные слова. Избегать специальных слов для животных, если они отличаются. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic intransitive verb for swift motion of human beings with the feet. Avoid terms meaning "function", "manage" etc.. Avoid terms for movement of e.g. liquids, where different. Avoid terms specifically for animals, where different. (CoBL)</t>
+    <t xml:space="preserve">Most generic intransitive verb for swift motion of human beings with the feet. Avoid terms meaning “function”, “manage” etc.. Avoid terms for movement of e.g. liquids, where different. Avoid terms specifically for animals, where different. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Ты умеешь быстро бегать? (CoBL) 2. По песку трудно бежать.</t>
@@ -15230,7 +15230,7 @@
     <t xml:space="preserve">Самый общий глагол, обозначающий положение человека в покое с выпрямленной спиной на ногах. (см. далее CoBL) Во многих языках стативный глагол ‘стоять’ отсутствует. Тогда следует заполнять это значение инхоативным глаголом.</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for standing in its basic sense of a person being in an upright position on their feet.  Of a person, i.e. not of a building 'standing' or being in a place.  Not a location meaning, i.e. not 'stand' in the sense of 'be in a place', e.g. not 'estar' in Spanish -- the correct Spanish lexeme choice is estar parado.  Stative meaning, 'be standing', rather than change of state "stand up", "get up", Spanish pararse. (CoBL) Many languages lack a durative verb of standing altogether. In these languages, this meaning should be filled by an inchoative verb.</t>
+    <t xml:space="preserve">Most generic verb for standing in its basic sense of a person being in an upright position on their feet.  Of a person, i.e. not of a building ‘standing’ or being in a place.  Not a location meaning, i.e. not ‘stand’ in the sense of ‘be in a place’, e.g. not ‘estar’ in Spanish -- the correct Spanish lexeme choice is &lt;i&gt;estar parado&lt;/i&gt;.  Stative meaning, ‘be standing’, rather than change of state “stand up”, “get up”, Spanish &lt;i&gt;pararse&lt;/i&gt;. (CoBL) Many languages lack a durative verb of standing altogether. In these languages, this meaning should be filled by an inchoative verb.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Человек может стоять, сидеть и лежать. (GLD) 2. Он стоит на двух ногах. (GLD) 3. Я устал стоять, я хочу лечь. (GLD)</t>
@@ -15674,7 +15674,7 @@
     <t xml:space="preserve">Самое общее слово, как правило, наречие, обозначающее пространственную близость. Избегать прилагательных и послелогов, если они отличаются. Избегать слов для ‘по соседству’, ‘около’ и т.д. Антоним ДАЛЕКО. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic word, typically adverbial, indicating proximity. Avoid adjectives, if different, e.g. "nearby". Avoid dedicated adpositions, e.g. "near (to) the river". Avoid terms for "adjacent", "next to" etc. Antonym of "far (away)". (CoBL)</t>
+    <t xml:space="preserve">Most generic word, typically adverbial, indicating proximity. Avoid adjectives, if different, e.g. “nearby”. Avoid dedicated adpositions, e.g. “near (to) the river”. Avoid terms for “adjacent”, “next to” etc. Antonym of “far (away)”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Это дерево далеко, я его плохо вижу, а это дерево близко, я его хорошо вижу. (GLD) 2. Туда можно дойти за один день, это близко. (CoBL)</t>
@@ -15692,7 +15692,7 @@
     <t xml:space="preserve">Самое общее слово, как правило, наречие, обозначающее высокую степень удалённости в пространстве. Избегать прилагательных и послелогов, если они отличаются. Антоним БЛИЗКО. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic word, typically adverbial, indicating distance from a point of reference. Avoid adjectives, if different, e.g. "distant, remote". (Some languages with large adjectival classes may derive words for "far" from an adjective.) Avoid dedicated adpositions. Avoid compound expressions, "far away", unless really the most basic term. Antonym of "near". (CoBL)</t>
+    <t xml:space="preserve">Most generic word, typically adverbial, indicating distance from a point of reference. Avoid adjectives, if different, e.g. “distant, remote”. (Some languages with large adjectival classes may derive words for “far” from an adjective.) Avoid dedicated adpositions. Avoid compound expressions, “far away”, unless really the most basic term. Antonym of “near”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он далеко, он меня не слышит. 2. Это дерево далеко, я его плохо вижу, а это дерево близко, я его хорошо вижу. (GLD)</t>
@@ -15776,7 +15776,7 @@
     <t xml:space="preserve">Антоним «маленького». Самый общий термин, как правило, прилагательное, относящийся к большому размеру неодушевлённого объекта.</t>
   </si>
   <si>
-    <t xml:space="preserve">The antonym of "small". Most generic term, typically adjectival, referring to the physical largeness of size of an inanimate object. (CoBL)</t>
+    <t xml:space="preserve">The antonym of “small”. Most generic term, typically adjectival, referring to the physical largeness of size of an inanimate object. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Муравей очень маленький. 2. Этот камень большой, а тот — маленький.</t>
@@ -15794,7 +15794,7 @@
     <t xml:space="preserve">Антоним «большого». Самое общее слово, как правило, прилагательное, относящееся к малому физическому размеру неодушевлённого предмета. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">The antonym of "big". The most generic term, typically adjectival, referring to the physical smallness of size of inanimate object. (CoBL)</t>
+    <t xml:space="preserve">The antonym of “big”. The most generic term, typically adjectival, referring to the physical smallness of size of inanimate object. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. У этого человека большой нос, а у того — маленький. (GLD) 2. Это большой камень, а это — маленький. (CoBL)</t>
@@ -15962,7 +15962,7 @@
     <t xml:space="preserve">Самое общее прилагательное, описывающее путь прямой, не изогнутой линии. (далее см. CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term describing the path of an uncurved line. Avoid terms specifically meaning "moral correctness" or "proper conduct". Avoid terms specifically meaning "straight ahead" in spatial directions (implying goal of motion). (CoBL)</t>
+    <t xml:space="preserve">Most generic term describing the path of an uncurved line. Avoid terms specifically meaning “moral correctness” or “proper conduct”. Avoid terms specifically meaning “straight ahead” in spatial directions (implying goal of motion). (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Эта палка прямая, а та — кривая. (CoBL) 2. От нашего селения до ХХ прямая дорога.</t>
@@ -16775,7 +16775,7 @@
     <t xml:space="preserve">Самое общее слово для относительно большого возраста неодушевлённого объекта. (далее см. CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic adjective for the relative age of an inanimate object. Avoid terms specifically for food, e.g. "rotten, gone off" etc., where different. Avoid terms for great age, e.g. "ancient", where different. Avoid terms applying to animates, e.g. "elderly, old man". Avoid terms indicating something is "worn out, thin" or no longer useful, e.g. for clothing. Avoid terms for "in ruins" etc. (CoBL)</t>
+    <t xml:space="preserve">Most generic adjective for the relative age of an inanimate object. Avoid terms specifically for food, e.g. “rotten, gone off” etc., where different. Avoid terms for great age, e.g. “ancient”, where different. Avoid terms applying to animates, e.g. “elderly, old man”. Avoid terms indicating something is “worn out, thin” or no longer useful, e.g. for clothing. Avoid terms for “in ruins” etc. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Он живёт в старом доме, а не в новом. (CoBL) 2. XX — очень старый город.</t>
@@ -16991,7 +16991,7 @@
     <t xml:space="preserve">Самое общее слово для светлого времени суток, в противовес ночи. Антоним слова НОЧЬ. Избегать слов для понятия ДЕНЬ, СУТКИ. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic term for the light period in contrast to night. Antonym of "night". Avoid terms referring to the "24-hour period". (CoBL)</t>
+    <t xml:space="preserve">Most generic term for the light period in contrast to night. Antonym of “night”. Avoid terms referring to the “24-hour period”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Ночь сменяет день. (GLD) 2. Сейчас день, надо работать.</t>
@@ -17384,7 +17384,7 @@
     <t xml:space="preserve">В соответствии с дефиницей CoBL, необходимо использовать глагол пассивного, а не активного восприятия запаха (‘чуять’, не ‘нюхать’); русский перевод выбран условно, т.к. в русском языке нет простого нейтрального глагола с таким значением (&lt;i&gt;чуять&lt;/i&gt; преимущественно используется о животных). Русское соответствие для этого глагола — &lt;i&gt;чувствовать запах&lt;/i&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">Perceiving an odour, by a human, through the nose. Not emitting an odour, smelling of something, e.g. by a flower. So not as in "the food smells good". The transitive verb (form) used where the subject of the verb is the person who perceives the odour, while that odour, or the substance or thing emitting it, is the object. Some languages (e.g. Slavic) have different verbs where the human subject is either the experiencer or agent of 'smell' (the same contrast that English itself has for other perception meanings such as 'see' vs. 'look', 'hear' vs. 'listen'). In such languages, select the verb form where the human subject is experiencer, not agent, who perceives the odour passively, not actively and intentionally 'sniffing' for it. So not as in "she knelt down and smelt the flowers".</t>
+    <t xml:space="preserve">Perceiving an odour, by a human, through the nose. Not emitting an odour, smelling of something, e.g. by a flower. So not as in “the food smells good”. The transitive verb (form) used where the subject of the verb is the person who perceives the odour, while that odour, or the substance or thing emitting it, is the object. Some languages (e.g. Slavic) have different verbs where the human subject is either the experiencer or agent of ‘smell’ (the same contrast that English itself has for other perception meanings such as ‘see’ vs. ‘look’, ‘hear’ vs. ‘listen’). In such languages, select the verb form where the human subject is experiencer, not agent, who perceives the odour passively, not actively and intentionally ‘sniffing’ for it. So not as in “she knelt down and smelt the flowers”.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Я чувствую / чую запах дыма. (CoBL) 2. Волк почуял запах человека.</t>
@@ -17528,7 +17528,7 @@
     <t xml:space="preserve">Самый общий непереходный глагол для пассивного восприятия ухом. Избегать активных слов, например, ‘слушать’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic transitive verb for perceiving something passively with the ear. Avoid active terms, e.g. "listen". (CoBL)</t>
+    <t xml:space="preserve">Most generic transitive verb for perceiving something passively with the ear. Avoid active terms, e.g. “listen”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Ты тихо говоришь, я тебя не слышу. 2. Я неожиданно услышал выстрел.</t>
@@ -17816,7 +17816,7 @@
     <t xml:space="preserve">Самое общее прилагательное, относящееся к сопротивлению твёрдой материи силе нажатия. Антоним понятия МЯГКИЙ. Избегать слов со значением ‘твёрдый’. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic adjective referring to the resistance of solid matter to compressive force. Antonym of SOFT. Avoid terms for "difficult". (CoBL)</t>
+    <t xml:space="preserve">Most generic adjective referring to the resistance of solid matter to compressive force. Antonym of SOFT. Avoid terms for “difficult”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Еда была очень жёсткой. Когда он её укусил, он сломал зуб. (CoBL) 2. Пол твёрдый, ковёр мягкий.</t>
@@ -17852,7 +17852,7 @@
     <t xml:space="preserve">Антоним понятия ТУПОЙ. Базовое слово, как правило, адъективное, относящееся к хорошей способности резать ножа или другого режущего предмета. Избегать слов, относящихся к остроте интеллекта. Избегать перцептивных терминов для вкуса, боли, зрения и т.д. (CoBL)</t>
   </si>
   <si>
-    <t xml:space="preserve">Antonym of "blunt/dull". Basic term, typically adjectival, referring to the good cutting ability of a knife or other cutting object. Avoid terms specifically for keenness of intelligence. Avoid perceptual terms for taste, pain, vision etc. (CoBL)</t>
+    <t xml:space="preserve">Antonym of “blunt/dull”. Basic term, typically adjectival, referring to the good cutting ability of a knife or other cutting object. Avoid terms specifically for keenness of intelligence. Avoid perceptual terms for taste, pain, vision etc. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">Острый нож режет лучше, чем тупой. (CoBL)</t>
@@ -17960,7 +17960,7 @@
     <t xml:space="preserve">Самое общее прилагательное, описывающее наличие воды, а не только влажности. Наличие воды в материале насквозь, не только на поверхности. Антоним понятия СУХОЙ. Избегать слов, относящихся специально к изменению состояния. Избегать интенсивных значений. Избегать специальных обозначений влажности воздуха. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic adjective describing presence of water, not merely moisture or humidity. Presence of water throughout a material, not just surface moisture. Antonym of "dry". Avoid terms specifically for change of state. Avoid intensive meanings, e.g. "soaked". Avoid terms specifically for humidity in the air. (CoBL)</t>
+    <t xml:space="preserve">Most generic adjective describing presence of water, not merely moisture or humidity. Presence of water throughout a material, not just surface moisture. Antonym of “dry”. Avoid terms specifically for change of state. Avoid intensive meanings, e.g. “soaked”. Avoid terms specifically for humidity in the air. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Эта рубашка мокрая, сними её. 2. Этот камень мокрый, не сиди на нём. 3. Мокрая спичка не загорится, сухая загорится.</t>
@@ -18836,7 +18836,7 @@
     <t xml:space="preserve">Темпоральное вопросительное слово, относящееся к моменту времени, а не к длительности. Самая общая форма, избегать форм для, например, ‘в какой час?’. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Temporal, punctual not durative, interrogative. Most generic form, avoiding eliciting terms specifically for e.g. "at what hour?" (CoBL)</t>
+    <t xml:space="preserve">Temporal, punctual not durative, interrogative. Most generic form, avoiding eliciting terms specifically for e.g. “at what hour?” (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">Когда ты придёшь?</t>
@@ -18854,7 +18854,7 @@
     <t xml:space="preserve">Вопросительное местоимение в локативном эссивном значении (не ‘куда’ или ‘откуда’). (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Interrogative pronoun. Locative meaning. Static, i.e. not "whither" or "whence". (CoBL)</t>
+    <t xml:space="preserve">Interrogative pronoun. Locative meaning. Static, i.e. not “whither” or “whence”. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">Где ты живёшь?</t>
@@ -18926,7 +18926,7 @@
     <t xml:space="preserve">Вопросительное слово образа действия.</t>
   </si>
   <si>
-    <t xml:space="preserve">Interrogative of manner. Meaning "in what way/manner" rather than "in what state". Avoid elicitation with, e.g. "How are you?", How is the weather?" (CoBL)</t>
+    <t xml:space="preserve">Interrogative of manner. Meaning “in what way/manner” rather than “in what state”. Avoid elicitation with, e.g. “How are you?”, “How is the weather?” (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">Как разжечь костёр?</t>
@@ -18998,7 +18998,7 @@
     <t xml:space="preserve">Самый общий глагол для произнесения гармоничных звуков ртом. Избегать слов для ‘читать вслух’, ‘декларировать’, если они отличаются. (CoBL) </t>
   </si>
   <si>
-    <t xml:space="preserve">Most generic verb for producing harmonious sounds with the mouth. Avoid terms for "recite" etc., where different. (CoBL)</t>
+    <t xml:space="preserve">Most generic verb for producing harmonious sounds with the mouth. Avoid terms for “recite” etc., where different. (CoBL)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Она красиво поёт. 2. В мечети / церкви много поют.</t>
@@ -20285,8 +20285,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D150" activeCellId="0" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20298,7 +20298,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="209.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="1.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="167.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="210.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.48"/>

</xml_diff>

<commit_message>
Specified that the dove should be domestic.
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -3337,10 +3337,10 @@
     <t xml:space="preserve">DOVE</t>
   </si>
   <si>
-    <t xml:space="preserve">Птица семейства голубиных (&lt;i&gt;Columbidae&lt;/i&gt;). (Concepticon)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One of several birds of the family Columbidae.  (Concepticon)</t>
+    <t xml:space="preserve">Птица семейства голубиных (&lt;i&gt;Columbidae&lt;/i&gt;). (Concepticon) Когда возможно, выбирать слово для домашнего голубя (Columba livia domestica).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of several birds of the family Columbidae.  (Concepticon) When possible, choose the word for the domestic dove (&lt;i&gt;Columba livia domestica&lt;/i&gt;).</t>
   </si>
   <si>
     <t xml:space="preserve">1. Голубь ест остатки пищи. 2. Голуби людей не боятся.</t>
@@ -20257,8 +20257,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20285,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D150" activeCellId="0" sqref="D150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H178" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J184" activeCellId="0" sqref="J184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28444,7 +28448,7 @@
       <c r="H173" s="0" t="n">
         <v>1360</v>
       </c>
-      <c r="I173" s="0" t="s">
+      <c r="I173" s="1" t="s">
         <v>1039</v>
       </c>
       <c r="J173" s="0" t="s">
@@ -51502,7 +51506,7 @@
       <c r="I665" s="0" t="s">
         <v>3959</v>
       </c>
-      <c r="J665" s="1" t="s">
+      <c r="J665" s="2" t="s">
         <v>3960</v>
       </c>
       <c r="K665" s="0" t="s">

</xml_diff>

<commit_message>
clarified domestic vs wild duck
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -3139,10 +3139,10 @@
     <t xml:space="preserve">DUCK</t>
   </si>
   <si>
-    <t xml:space="preserve">Водоплавающая птица семейства утиных с плоским клювом и перепончатыми лапами. (Concepticon) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">An aquatic bird of the family Anatidae, having a flat bill and webbed feet. (Concepticon)</t>
+    <t xml:space="preserve">Водоплавающая птица семейства утиных с плоским клювом и перепончатыми лапами. (Concepticon) При наличии двух разных слов выбирать слово для домашней утки.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An aquatic bird of the family Anatidae, having a flat bill and webbed feet. (Concepticon) If two words are present, select the one for a domestic duck.</t>
   </si>
   <si>
     <t xml:space="preserve">Утки водятся на больших реках и озёрах.</t>
@@ -20289,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H178" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J184" activeCellId="0" sqref="J184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A158" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J173" activeCellId="0" sqref="J173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
clarified saliva as specifically saliva inside the mouth
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -6652,10 +6652,10 @@
     <t xml:space="preserve">SALIVA</t>
   </si>
   <si>
-    <t xml:space="preserve">Выделение слюнных желёз, которое можно выплюнуть. (Concepticon)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A secretion from the salivary glands (found in the mouth) that can be spat out. (Concepticon)</t>
+    <t xml:space="preserve">Выделение слюнных желёз, которое можно выплюнуть. (Concepticon) Если ‘слюна во рту’ и ‘слюна вне рта’ (‘плевок’) выражаются разными словами, выбирать слово со значением ‘слюна во рту’.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A secretion from the salivary glands (found in the mouth) that can be spat out. (Concepticon) If the words for ‘saliva inside mouth’ and ‘saliva outside mouth’ (‘spitful’) are different, choose the word with the meaning ‘saliva inside mouth’.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Во рту всегда бывает слюна. 2. Он выплюнул слюну изо рта.</t>
@@ -20289,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A158" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J173" activeCellId="0" sqref="J173"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C346" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J370" activeCellId="0" sqref="J370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
changed the context for 389 CORPSE (OF HUMAN)
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -7012,16 +7012,16 @@
     <t xml:space="preserve">CORPSE (OF HUMAN)</t>
   </si>
   <si>
-    <t xml:space="preserve">Тело мёртвого человека.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A dead person’s body.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. После боя на поле было много трупов. 2. Его труп похоронили.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. There were many bodies in the field after the battle. 2. His dead body was buried.</t>
+    <t xml:space="preserve">Тело мёртвого человека. Отличать от прилагательного, обозначающего ‘мёртвого’, ‘недавно умершего’ (ср.: ‘после боя на поле было много трупов’ ~ ‘после боя на поле было много погибших’).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A dead person’s body. To be distinguished from an adjective denoting ‘dead’, ‘recently deceased’ (cf.: ‘After the battle there were many bodies in the field’ ~ ‘After the battle there were many dead in the field’).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Трупы надо закапывать в землю. 2. Его труп похоронили.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dead bodies must be buried in the earth. 2. His dead body was buried.</t>
   </si>
   <si>
     <t xml:space="preserve">ТУША (ЖИВОТНОГО)</t>
@@ -20289,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C346" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I375" activeCellId="0" sqref="I375"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A390" activeCellId="0" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
clarified definitions for 503 PUT ON (DRESS) and 506 REMOVE (DRESS)
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -9064,10 +9064,10 @@
     <t xml:space="preserve">PUT ON (DRESS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Надевать одежду, закрывающую верхнюю часть тела (рубашку, платье).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To put on clothing that covers the upper part of the body (shirt, dress).</t>
+    <t xml:space="preserve">Надевать одежду, закрывающую верхнюю часть тела (рубашку, платье). Если есть различие между рубашкой и платьем, выбирать слово, используемое для платья (в соответствии с обозначением лексемы).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To put on clothing that covers the upper part of the body (shirt, dress). If shirt and dress are different, choose the word for dress (in accordance with the headword).</t>
   </si>
   <si>
     <t xml:space="preserve">1. Я надел рубашку. 2. Она надела платье.</t>
@@ -9118,10 +9118,10 @@
     <t xml:space="preserve">REMOVE (DRESS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Снимать одежду, закрывающую верхнюю часть тела (рубашку, платье).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To remove clothing that covers the upper part of the body (shirt, dress). </t>
+    <t xml:space="preserve">Снимать одежду, закрывающую верхнюю часть тела (рубашку, платье). Если есть различие между рубашкой и платьем, выбирать слово, используемое для платья (в соответствии с обозначением лексемы).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To remove clothing that covers the upper part of the body (shirt, dress). If shirt and dress are different, choose the word for dress (in accordance with the headword).</t>
   </si>
   <si>
     <t xml:space="preserve">1. Я снял рубашку. 2. Она сняла платье.</t>
@@ -20289,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A390" activeCellId="0" sqref="A390"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A489" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J507" activeCellId="0" sqref="J507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
specified that butter should be melted
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -8938,10 +8938,10 @@
     <t xml:space="preserve">BUTTER</t>
   </si>
   <si>
-    <t xml:space="preserve">Твёрдое, жирное вещество, производимое сбиванием молочных сливок. (Concepticon)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A soft, fatty foodstuff that is made by churning the cream of milk (most often cows milk). (Concepticon)</t>
+    <t xml:space="preserve">Твёрдое, жирное вещество, производимое сбиванием молочных сливок. (Concepticon) В культурах Кавказа наименее маркированным обычно является топлёное масло, так что при наличии двух разных слов следует выбирать его.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A soft, fatty foodstuff that is made by churning the cream of milk (most often cows milk). (Concepticon) If there is a difference between ‘non-melted’ and ‘melted’ butter, choose the latter, as it is usually more common in the Caucasus.</t>
   </si>
   <si>
     <t xml:space="preserve">Масло взбивают из молока.</t>
@@ -20257,12 +20257,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20289,8 +20285,8 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A539" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A554" activeCellId="0" sqref="A554"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J497" activeCellId="0" sqref="J497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28448,7 +28444,7 @@
       <c r="H173" s="0" t="n">
         <v>1360</v>
       </c>
-      <c r="I173" s="1" t="s">
+      <c r="I173" s="0" t="s">
         <v>1039</v>
       </c>
       <c r="J173" s="0" t="s">
@@ -51506,7 +51502,7 @@
       <c r="I665" s="0" t="s">
         <v>3959</v>
       </c>
-      <c r="J665" s="2" t="s">
+      <c r="J665" s="1" t="s">
         <v>3960</v>
       </c>
       <c r="K665" s="0" t="s">

</xml_diff>

<commit_message>
fixed def for DOGWOOD
</commit_message>
<xml_diff>
--- a/templates/lexcauc-concepts.xlsx
+++ b/templates/lexcauc-concepts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -11902,8 +11902,7 @@
     <t xml:space="preserve">Кислый, красный плод растения рода Кизил (Cornus) грушевидной формы.</t>
   </si>
   <si>
-    <t xml:space="preserve">Плод растения рода Кизил (Cornus), с кислыми красными плодами грушевидной формы. 
-A pear-shaped, red, sour fruit of a plant of the genus Cornus.</t>
+    <t xml:space="preserve">Плод растения рода Кизил (Cornus), с кислыми красными плодами грушевидной формы.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Барбарис меньше кизила. 2. Кизил кислый.</t>
@@ -20198,6 +20197,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -20285,15 +20285,15 @@
   </sheetPr>
   <dimension ref="A1:Q1133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J497" activeCellId="0" sqref="J497"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A659" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E673" activeCellId="0" sqref="E673"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="4.07"/>
@@ -20305,7 +20305,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51477,7 +51477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="665" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="665" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="n">
         <v>664</v>
       </c>

</xml_diff>